<commit_message>
Finished Chinese rulebook and updated rulebook
</commit_message>
<xml_diff>
--- a/OrganicChemistryBoardGame v2.1 w extra.xlsx
+++ b/OrganicChemistryBoardGame v2.1 w extra.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Barry\Organic Chemistry Board Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B96682-BC15-495C-9306-75DCC35BAD98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A44DCEFA-CF22-4950-A9DF-16C522181C3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="441">
   <si>
     <t>Image</t>
   </si>
@@ -83,33 +83,18 @@
     <t>LDA</t>
   </si>
   <si>
-    <t>LiAlH4</t>
-  </si>
-  <si>
     <t>mCPBA</t>
   </si>
   <si>
     <t>MsCl</t>
   </si>
   <si>
-    <t>NaBH4</t>
-  </si>
-  <si>
     <t>NBS</t>
   </si>
   <si>
     <t>NCS</t>
   </si>
   <si>
-    <t>NH2OH</t>
-  </si>
-  <si>
-    <t>OsO4</t>
-  </si>
-  <si>
-    <t>PCl3</t>
-  </si>
-  <si>
     <t>TsCl</t>
   </si>
   <si>
@@ -170,9 +155,6 @@
     <t>Propene</t>
   </si>
   <si>
-    <t>DMF (N,N Dimethyl formamide)</t>
-  </si>
-  <si>
     <t>Acetonitrile</t>
   </si>
   <si>
@@ -206,27 +188,15 @@
     <t>乙酰氯</t>
   </si>
   <si>
-    <t>KMnO4</t>
-  </si>
-  <si>
     <t>Pd/C</t>
   </si>
   <si>
     <t>Pt</t>
   </si>
   <si>
-    <t>CrO3</t>
-  </si>
-  <si>
-    <t>SeO2</t>
-  </si>
-  <si>
     <t>Ra-Ni</t>
   </si>
   <si>
-    <t>HIO4</t>
-  </si>
-  <si>
     <t>Lindler's catalyst</t>
   </si>
   <si>
@@ -236,33 +206,6 @@
     <t>Mg</t>
   </si>
   <si>
-    <t>O3</t>
-  </si>
-  <si>
-    <t>B2H6</t>
-  </si>
-  <si>
-    <t>H2O2</t>
-  </si>
-  <si>
-    <t>N2H4</t>
-  </si>
-  <si>
-    <t>MnO2</t>
-  </si>
-  <si>
-    <t>NaClO2</t>
-  </si>
-  <si>
-    <t>Pb(OAc)4</t>
-  </si>
-  <si>
-    <t>HNO3</t>
-  </si>
-  <si>
-    <t>K2CO3</t>
-  </si>
-  <si>
     <t>DBU</t>
   </si>
   <si>
@@ -281,42 +224,15 @@
     <t>n-BuLi</t>
   </si>
   <si>
-    <t>NaNH2</t>
-  </si>
-  <si>
-    <t>H2</t>
-  </si>
-  <si>
     <t>CO</t>
   </si>
   <si>
-    <t>H2O</t>
-  </si>
-  <si>
     <t>Urea</t>
   </si>
   <si>
-    <t>Br2</t>
-  </si>
-  <si>
-    <t>Cl2</t>
-  </si>
-  <si>
-    <t>I2</t>
-  </si>
-  <si>
     <t>KI</t>
   </si>
   <si>
-    <t>PPh3</t>
-  </si>
-  <si>
-    <t>NaN3</t>
-  </si>
-  <si>
-    <t>CO2</t>
-  </si>
-  <si>
     <t>Ethylene glycol</t>
   </si>
   <si>
@@ -324,12 +240,6 @@
   </si>
   <si>
     <t>hv</t>
-  </si>
-  <si>
-    <t>BF3</t>
-  </si>
-  <si>
-    <t>CeCl3</t>
   </si>
   <si>
     <t>NIS</t>
@@ -784,9 +694,6 @@
     <t>v2\Reagents\Ag2O.png</t>
   </si>
   <si>
-    <t>H2SO4</t>
-  </si>
-  <si>
     <t>硫酸</t>
   </si>
   <si>
@@ -841,18 +748,9 @@
     <t>丁二烯</t>
   </si>
   <si>
-    <t>Ag2O</t>
-  </si>
-  <si>
     <t>Zn (Or any Zn alloy)</t>
   </si>
   <si>
-    <t>POCl3</t>
-  </si>
-  <si>
-    <t>H3PO4</t>
-  </si>
-  <si>
     <t>v2\Reagents\CH2N2.png</t>
   </si>
   <si>
@@ -866,9 +764,6 @@
   </si>
   <si>
     <t>DMP</t>
-  </si>
-  <si>
-    <t>H2CrO4</t>
   </si>
   <si>
     <t>PCC</t>
@@ -913,12 +808,6 @@
     <t>DIBAL</t>
   </si>
   <si>
-    <t>LiAlH(OtBu)3</t>
-  </si>
-  <si>
-    <t>Ni2B</t>
-  </si>
-  <si>
     <t>氢化二异丁基铝溶液</t>
   </si>
   <si>
@@ -987,18 +876,6 @@
     <t>v2\Templates\Base.png</t>
   </si>
   <si>
-    <t>PBr3</t>
-  </si>
-  <si>
-    <t>PCl5</t>
-  </si>
-  <si>
-    <t>SOBr2</t>
-  </si>
-  <si>
-    <t>SOCl2</t>
-  </si>
-  <si>
     <t>三溴化磷</t>
   </si>
   <si>
@@ -1086,18 +963,12 @@
     <t>v2\Templates\RXN COND &amp; H2O.png</t>
   </si>
   <si>
-    <t>CH2N2</t>
-  </si>
-  <si>
     <t>DCC</t>
   </si>
   <si>
     <t>KCN</t>
   </si>
   <si>
-    <t>P2O5</t>
-  </si>
-  <si>
     <t>二环己基碳二亚胺</t>
   </si>
   <si>
@@ -1122,27 +993,18 @@
     <t>v2\Templates\Other.png</t>
   </si>
   <si>
-    <t>NaIO4</t>
-  </si>
-  <si>
     <t>高碘酸钠</t>
   </si>
   <si>
     <t>v2\Reagents\NaIO4.png</t>
   </si>
   <si>
-    <t>Hg(OAc)2</t>
-  </si>
-  <si>
     <t>醋酸汞</t>
   </si>
   <si>
     <t>v2\Reagents\Hg(OAc)2.png</t>
   </si>
   <si>
-    <t>HgSO4</t>
-  </si>
-  <si>
     <t>硫酸汞</t>
   </si>
   <si>
@@ -1435,24 +1297,154 @@
   </si>
   <si>
     <t>v2\Products\v2\Image\13.png</t>
+  </si>
+  <si>
+    <t>Ag₂O</t>
+  </si>
+  <si>
+    <t>CrO₃</t>
+  </si>
+  <si>
+    <t>H₂CrO₄</t>
+  </si>
+  <si>
+    <t>H₂O₂</t>
+  </si>
+  <si>
+    <t>Hg(OAc)₂</t>
+  </si>
+  <si>
+    <t>HgSO₄</t>
+  </si>
+  <si>
+    <t>KMnO₄</t>
+  </si>
+  <si>
+    <t>MnO₂</t>
+  </si>
+  <si>
+    <t>NaClO₂</t>
+  </si>
+  <si>
+    <t>NaIO₄</t>
+  </si>
+  <si>
+    <t>O₃</t>
+  </si>
+  <si>
+    <t>OsO₄</t>
+  </si>
+  <si>
+    <t>Pb(OAc)₄</t>
+  </si>
+  <si>
+    <t>SeO₂</t>
+  </si>
+  <si>
+    <t>B₂H₆</t>
+  </si>
+  <si>
+    <t>CeCl₃</t>
+  </si>
+  <si>
+    <t>H₂</t>
+  </si>
+  <si>
+    <t>LiAlH(OtBu)₃</t>
+  </si>
+  <si>
+    <t>LiAlH₄</t>
+  </si>
+  <si>
+    <t>NaBH₄</t>
+  </si>
+  <si>
+    <t>Ni₂B</t>
+  </si>
+  <si>
+    <t>H₂SO₄</t>
+  </si>
+  <si>
+    <t>H₃PO₄</t>
+  </si>
+  <si>
+    <t>HIO₄</t>
+  </si>
+  <si>
+    <t>HNO₃</t>
+  </si>
+  <si>
+    <t>NaNH₂</t>
+  </si>
+  <si>
+    <t>K₂CO₃</t>
+  </si>
+  <si>
+    <t>Br₂</t>
+  </si>
+  <si>
+    <t>Cl₂</t>
+  </si>
+  <si>
+    <t>I₂</t>
+  </si>
+  <si>
+    <t>PBr₃</t>
+  </si>
+  <si>
+    <t>PCl₃</t>
+  </si>
+  <si>
+    <t>PCl₅</t>
+  </si>
+  <si>
+    <t>SOBr₂</t>
+  </si>
+  <si>
+    <t>SOCl₂</t>
+  </si>
+  <si>
+    <t>PPh₃</t>
+  </si>
+  <si>
+    <t>NaN₃</t>
+  </si>
+  <si>
+    <t>H₂O</t>
+  </si>
+  <si>
+    <t>BF₃</t>
+  </si>
+  <si>
+    <t>CH₂N₂</t>
+  </si>
+  <si>
+    <t>CO₂</t>
+  </si>
+  <si>
+    <t>N₂H₄</t>
+  </si>
+  <si>
+    <t>NH₂OH</t>
+  </si>
+  <si>
+    <t>P₂O₅</t>
+  </si>
+  <si>
+    <t>POCl₃</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1501,16 +1493,18 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1793,8 +1787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I212"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G96" sqref="G96:G106"/>
+    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A106" sqref="A106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1832,20 +1826,20 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>34</v>
+      <c r="A2" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>160</v>
+        <v>130</v>
       </c>
       <c r="D2" t="s">
-        <v>257</v>
+        <v>223</v>
       </c>
       <c r="E2" t="s">
-        <v>414</v>
+        <v>368</v>
       </c>
       <c r="F2" t="s">
         <v>12</v>
@@ -1855,20 +1849,20 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>35</v>
+      <c r="A3" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>161</v>
+        <v>131</v>
       </c>
       <c r="D3" t="s">
-        <v>257</v>
+        <v>223</v>
       </c>
       <c r="E3" t="s">
-        <v>414</v>
+        <v>368</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
@@ -1878,20 +1872,20 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>36</v>
+      <c r="A4" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>162</v>
+        <v>132</v>
       </c>
       <c r="D4" t="s">
-        <v>257</v>
+        <v>223</v>
       </c>
       <c r="E4" t="s">
-        <v>414</v>
+        <v>368</v>
       </c>
       <c r="F4" t="s">
         <v>12</v>
@@ -1900,21 +1894,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>37</v>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>250</v>
+        <v>219</v>
       </c>
       <c r="C5" t="s">
-        <v>163</v>
+        <v>133</v>
       </c>
       <c r="D5" t="s">
-        <v>257</v>
+        <v>223</v>
       </c>
       <c r="E5" t="s">
-        <v>414</v>
+        <v>368</v>
       </c>
       <c r="F5" t="s">
         <v>12</v>
@@ -1923,21 +1917,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>38</v>
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C6" t="s">
-        <v>164</v>
+        <v>134</v>
       </c>
       <c r="D6" t="s">
-        <v>257</v>
+        <v>223</v>
       </c>
       <c r="E6" t="s">
-        <v>414</v>
+        <v>368</v>
       </c>
       <c r="F6" t="s">
         <v>12</v>
@@ -1947,20 +1941,20 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>85</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>139</v>
+      <c r="A7" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>109</v>
       </c>
       <c r="C7" t="s">
-        <v>165</v>
+        <v>135</v>
       </c>
       <c r="D7" t="s">
-        <v>257</v>
+        <v>223</v>
       </c>
       <c r="E7" t="s">
-        <v>414</v>
+        <v>368</v>
       </c>
       <c r="F7" t="s">
         <v>12</v>
@@ -1969,21 +1963,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>39</v>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C8" t="s">
-        <v>166</v>
+        <v>136</v>
       </c>
       <c r="D8" t="s">
-        <v>257</v>
+        <v>223</v>
       </c>
       <c r="E8" t="s">
-        <v>414</v>
+        <v>368</v>
       </c>
       <c r="F8" t="s">
         <v>12</v>
@@ -1992,21 +1986,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>40</v>
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C9" t="s">
-        <v>167</v>
+        <v>137</v>
       </c>
       <c r="D9" t="s">
-        <v>257</v>
+        <v>223</v>
       </c>
       <c r="E9" t="s">
-        <v>414</v>
+        <v>368</v>
       </c>
       <c r="F9" t="s">
         <v>12</v>
@@ -2015,21 +2009,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>41</v>
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C10" t="s">
-        <v>168</v>
+        <v>138</v>
       </c>
       <c r="D10" t="s">
-        <v>257</v>
+        <v>223</v>
       </c>
       <c r="E10" t="s">
-        <v>414</v>
+        <v>368</v>
       </c>
       <c r="F10" t="s">
         <v>12</v>
@@ -2039,20 +2033,20 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>42</v>
+      <c r="A11" s="6" t="s">
+        <v>37</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>169</v>
+        <v>139</v>
       </c>
       <c r="D11" t="s">
-        <v>257</v>
+        <v>223</v>
       </c>
       <c r="E11" t="s">
-        <v>414</v>
+        <v>368</v>
       </c>
       <c r="F11" t="s">
         <v>12</v>
@@ -2062,20 +2056,20 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>43</v>
+      <c r="A12" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>170</v>
+        <v>140</v>
       </c>
       <c r="D12" t="s">
-        <v>257</v>
+        <v>223</v>
       </c>
       <c r="E12" t="s">
-        <v>414</v>
+        <v>368</v>
       </c>
       <c r="F12" t="s">
         <v>12</v>
@@ -2085,20 +2079,20 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>44</v>
+      <c r="A13" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="B13" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>171</v>
+        <v>141</v>
       </c>
       <c r="D13" t="s">
-        <v>257</v>
+        <v>223</v>
       </c>
       <c r="E13" t="s">
-        <v>414</v>
+        <v>368</v>
       </c>
       <c r="F13" t="s">
         <v>12</v>
@@ -2107,21 +2101,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>45</v>
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>39</v>
       </c>
       <c r="B14" t="s">
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>172</v>
+        <v>142</v>
       </c>
       <c r="D14" t="s">
-        <v>257</v>
+        <v>223</v>
       </c>
       <c r="E14" t="s">
-        <v>414</v>
+        <v>368</v>
       </c>
       <c r="F14" t="s">
         <v>12</v>
@@ -2130,21 +2124,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>46</v>
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>40</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>173</v>
+        <v>143</v>
       </c>
       <c r="D15" t="s">
-        <v>257</v>
+        <v>223</v>
       </c>
       <c r="E15" t="s">
-        <v>414</v>
+        <v>368</v>
       </c>
       <c r="F15" t="s">
         <v>12</v>
@@ -2153,21 +2147,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>47</v>
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>41</v>
       </c>
       <c r="B16" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C16" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="D16" t="s">
-        <v>257</v>
+        <v>223</v>
       </c>
       <c r="E16" t="s">
-        <v>414</v>
+        <v>368</v>
       </c>
       <c r="F16" t="s">
         <v>12</v>
@@ -2177,20 +2171,20 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>48</v>
+      <c r="A17" s="6" t="s">
+        <v>42</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C17" t="s">
-        <v>175</v>
+        <v>145</v>
       </c>
       <c r="D17" t="s">
-        <v>257</v>
+        <v>223</v>
       </c>
       <c r="E17" t="s">
-        <v>414</v>
+        <v>368</v>
       </c>
       <c r="F17" t="s">
         <v>12</v>
@@ -2200,20 +2194,20 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>251</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>262</v>
+      <c r="A18" s="6" t="s">
+        <v>396</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>227</v>
       </c>
       <c r="C18" t="s">
-        <v>231</v>
+        <v>201</v>
       </c>
       <c r="D18" t="s">
-        <v>256</v>
+        <v>222</v>
       </c>
       <c r="E18" t="s">
-        <v>281</v>
+        <v>244</v>
       </c>
       <c r="F18" t="s">
         <v>12</v>
@@ -2223,20 +2217,20 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>59</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>105</v>
+      <c r="A19" s="6" t="s">
+        <v>397</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="C19" t="s">
-        <v>179</v>
+        <v>149</v>
       </c>
       <c r="D19" t="s">
-        <v>256</v>
+        <v>222</v>
       </c>
       <c r="E19" t="s">
-        <v>281</v>
+        <v>244</v>
       </c>
       <c r="F19" t="s">
         <v>12</v>
@@ -2246,20 +2240,20 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>259</v>
+      <c r="A20" s="6" t="s">
+        <v>225</v>
       </c>
       <c r="B20" t="s">
-        <v>263</v>
+        <v>228</v>
       </c>
       <c r="C20" t="s">
-        <v>264</v>
+        <v>229</v>
       </c>
       <c r="D20" t="s">
-        <v>256</v>
+        <v>222</v>
       </c>
       <c r="E20" t="s">
-        <v>281</v>
+        <v>244</v>
       </c>
       <c r="F20" t="s">
         <v>12</v>
@@ -2269,20 +2263,20 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>260</v>
+      <c r="A21" s="6" t="s">
+        <v>398</v>
       </c>
       <c r="B21" t="s">
-        <v>267</v>
+        <v>232</v>
       </c>
       <c r="C21" t="s">
-        <v>265</v>
+        <v>230</v>
       </c>
       <c r="D21" t="s">
-        <v>256</v>
+        <v>222</v>
       </c>
       <c r="E21" t="s">
-        <v>281</v>
+        <v>244</v>
       </c>
       <c r="F21" t="s">
         <v>12</v>
@@ -2292,20 +2286,20 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>68</v>
+      <c r="A22" s="6" t="s">
+        <v>399</v>
       </c>
       <c r="B22" t="s">
-        <v>117</v>
+        <v>87</v>
       </c>
       <c r="C22" t="s">
-        <v>191</v>
+        <v>161</v>
       </c>
       <c r="D22" t="s">
-        <v>256</v>
+        <v>222</v>
       </c>
       <c r="E22" t="s">
-        <v>281</v>
+        <v>244</v>
       </c>
       <c r="F22" t="s">
         <v>12</v>
@@ -2315,20 +2309,20 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>340</v>
+      <c r="A23" s="6" t="s">
+        <v>400</v>
       </c>
       <c r="B23" t="s">
-        <v>341</v>
+        <v>296</v>
       </c>
       <c r="C23" t="s">
-        <v>342</v>
+        <v>297</v>
       </c>
       <c r="D23" t="s">
-        <v>256</v>
+        <v>222</v>
       </c>
       <c r="E23" t="s">
-        <v>281</v>
+        <v>244</v>
       </c>
       <c r="F23" t="s">
         <v>12</v>
@@ -2338,20 +2332,20 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>343</v>
+      <c r="A24" s="6" t="s">
+        <v>401</v>
       </c>
       <c r="B24" t="s">
-        <v>344</v>
+        <v>298</v>
       </c>
       <c r="C24" t="s">
-        <v>345</v>
+        <v>299</v>
       </c>
       <c r="D24" t="s">
-        <v>256</v>
+        <v>222</v>
       </c>
       <c r="E24" t="s">
-        <v>281</v>
+        <v>244</v>
       </c>
       <c r="F24" t="s">
         <v>12</v>
@@ -2361,20 +2355,20 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>56</v>
+      <c r="A25" s="6" t="s">
+        <v>402</v>
       </c>
       <c r="B25" t="s">
-        <v>102</v>
+        <v>72</v>
       </c>
       <c r="C25" t="s">
-        <v>176</v>
+        <v>146</v>
       </c>
       <c r="D25" t="s">
-        <v>256</v>
+        <v>222</v>
       </c>
       <c r="E25" t="s">
-        <v>281</v>
+        <v>244</v>
       </c>
       <c r="F25" t="s">
         <v>12</v>
@@ -2384,20 +2378,20 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>16</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>116</v>
+      <c r="A26" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="C26" t="s">
-        <v>189</v>
+        <v>159</v>
       </c>
       <c r="D26" t="s">
-        <v>256</v>
+        <v>222</v>
       </c>
       <c r="E26" t="s">
-        <v>281</v>
+        <v>244</v>
       </c>
       <c r="F26" t="s">
         <v>12</v>
@@ -2407,20 +2401,20 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>70</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>120</v>
+      <c r="A27" s="6" t="s">
+        <v>403</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="C27" t="s">
-        <v>194</v>
+        <v>164</v>
       </c>
       <c r="D27" t="s">
-        <v>256</v>
+        <v>222</v>
       </c>
       <c r="E27" t="s">
-        <v>281</v>
+        <v>244</v>
       </c>
       <c r="F27" t="s">
         <v>12</v>
@@ -2430,20 +2424,20 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>71</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>121</v>
+      <c r="A28" s="6" t="s">
+        <v>404</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="C28" t="s">
-        <v>195</v>
+        <v>165</v>
       </c>
       <c r="D28" t="s">
-        <v>256</v>
+        <v>222</v>
       </c>
       <c r="E28" t="s">
-        <v>281</v>
+        <v>244</v>
       </c>
       <c r="F28" t="s">
         <v>12</v>
@@ -2453,20 +2447,20 @@
       </c>
     </row>
     <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>337</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>338</v>
+      <c r="A29" s="6" t="s">
+        <v>405</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>294</v>
       </c>
       <c r="C29" t="s">
-        <v>339</v>
+        <v>295</v>
       </c>
       <c r="D29" t="s">
-        <v>256</v>
+        <v>222</v>
       </c>
       <c r="E29" t="s">
-        <v>281</v>
+        <v>244</v>
       </c>
       <c r="F29" t="s">
         <v>12</v>
@@ -2476,20 +2470,20 @@
       </c>
     </row>
     <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>66</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>112</v>
+      <c r="A30" s="6" t="s">
+        <v>406</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="C30" t="s">
-        <v>185</v>
+        <v>155</v>
       </c>
       <c r="D30" t="s">
-        <v>256</v>
+        <v>222</v>
       </c>
       <c r="E30" t="s">
-        <v>281</v>
+        <v>244</v>
       </c>
       <c r="F30" t="s">
         <v>12</v>
@@ -2499,20 +2493,20 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>22</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>119</v>
+      <c r="A31" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="C31" t="s">
-        <v>193</v>
+        <v>163</v>
       </c>
       <c r="D31" t="s">
-        <v>256</v>
+        <v>222</v>
       </c>
       <c r="E31" t="s">
-        <v>281</v>
+        <v>244</v>
       </c>
       <c r="F31" t="s">
         <v>12</v>
@@ -2522,20 +2516,20 @@
       </c>
     </row>
     <row r="32" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>72</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>268</v>
+      <c r="A32" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>233</v>
       </c>
       <c r="C32" t="s">
-        <v>196</v>
+        <v>166</v>
       </c>
       <c r="D32" t="s">
-        <v>256</v>
+        <v>222</v>
       </c>
       <c r="E32" t="s">
-        <v>281</v>
+        <v>244</v>
       </c>
       <c r="F32" t="s">
         <v>12</v>
@@ -2545,20 +2539,20 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>261</v>
+      <c r="A33" s="6" t="s">
+        <v>226</v>
       </c>
       <c r="B33" t="s">
-        <v>269</v>
+        <v>234</v>
       </c>
       <c r="C33" t="s">
-        <v>266</v>
+        <v>231</v>
       </c>
       <c r="D33" t="s">
-        <v>256</v>
+        <v>222</v>
       </c>
       <c r="E33" t="s">
-        <v>281</v>
+        <v>244</v>
       </c>
       <c r="F33" t="s">
         <v>12</v>
@@ -2568,20 +2562,20 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>60</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>106</v>
+      <c r="A34" s="6" t="s">
+        <v>409</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="C34" t="s">
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="D34" t="s">
-        <v>256</v>
+        <v>222</v>
       </c>
       <c r="E34" t="s">
-        <v>281</v>
+        <v>244</v>
       </c>
       <c r="F34" t="s">
         <v>12</v>
@@ -2591,20 +2585,20 @@
       </c>
     </row>
     <row r="35" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>67</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>115</v>
+      <c r="A35" s="6" t="s">
+        <v>410</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="C35" t="s">
-        <v>188</v>
+        <v>158</v>
       </c>
       <c r="D35" t="s">
-        <v>279</v>
+        <v>242</v>
       </c>
       <c r="E35" t="s">
-        <v>280</v>
+        <v>243</v>
       </c>
       <c r="F35" t="s">
         <v>12</v>
@@ -2614,20 +2608,20 @@
       </c>
     </row>
     <row r="36" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>97</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>158</v>
+      <c r="A36" s="6" t="s">
+        <v>411</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="C36" t="s">
-        <v>228</v>
+        <v>198</v>
       </c>
       <c r="D36" t="s">
-        <v>279</v>
+        <v>242</v>
       </c>
       <c r="E36" t="s">
-        <v>280</v>
+        <v>243</v>
       </c>
       <c r="F36" t="s">
         <v>12</v>
@@ -2637,20 +2631,20 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>270</v>
+      <c r="A37" s="6" t="s">
+        <v>235</v>
       </c>
       <c r="B37" t="s">
-        <v>273</v>
+        <v>236</v>
       </c>
       <c r="C37" t="s">
-        <v>274</v>
+        <v>237</v>
       </c>
       <c r="D37" t="s">
-        <v>279</v>
+        <v>242</v>
       </c>
       <c r="E37" t="s">
-        <v>280</v>
+        <v>243</v>
       </c>
       <c r="F37" t="s">
         <v>12</v>
@@ -2660,20 +2654,20 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>82</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>136</v>
+      <c r="A38" s="6" t="s">
+        <v>412</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>106</v>
       </c>
       <c r="C38" t="s">
-        <v>206</v>
+        <v>176</v>
       </c>
       <c r="D38" t="s">
-        <v>279</v>
+        <v>242</v>
       </c>
       <c r="E38" t="s">
-        <v>280</v>
+        <v>243</v>
       </c>
       <c r="F38" t="s">
         <v>12</v>
@@ -2682,21 +2676,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>271</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>277</v>
+    <row r="39" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>413</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>240</v>
       </c>
       <c r="C39" t="s">
-        <v>275</v>
+        <v>238</v>
       </c>
       <c r="D39" t="s">
-        <v>279</v>
+        <v>242</v>
       </c>
       <c r="E39" t="s">
-        <v>280</v>
+        <v>243</v>
       </c>
       <c r="F39" t="s">
         <v>12</v>
@@ -2706,20 +2700,20 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>15</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>114</v>
+      <c r="A40" s="6" t="s">
+        <v>414</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="C40" t="s">
-        <v>187</v>
+        <v>157</v>
       </c>
       <c r="D40" t="s">
-        <v>279</v>
+        <v>242</v>
       </c>
       <c r="E40" t="s">
-        <v>280</v>
+        <v>243</v>
       </c>
       <c r="F40" t="s">
         <v>12</v>
@@ -2728,21 +2722,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>63</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>109</v>
+    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="C41" t="s">
-        <v>230</v>
+        <v>200</v>
       </c>
       <c r="D41" t="s">
-        <v>279</v>
+        <v>242</v>
       </c>
       <c r="E41" t="s">
-        <v>280</v>
+        <v>243</v>
       </c>
       <c r="F41" t="s">
         <v>12</v>
@@ -2752,20 +2746,20 @@
       </c>
     </row>
     <row r="42" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>18</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>113</v>
+      <c r="A42" s="6" t="s">
+        <v>415</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="C42" t="s">
-        <v>186</v>
+        <v>156</v>
       </c>
       <c r="D42" t="s">
-        <v>279</v>
+        <v>242</v>
       </c>
       <c r="E42" t="s">
-        <v>280</v>
+        <v>243</v>
       </c>
       <c r="F42" t="s">
         <v>12</v>
@@ -2775,20 +2769,20 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>272</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>278</v>
+      <c r="A43" s="6" t="s">
+        <v>416</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>241</v>
       </c>
       <c r="C43" t="s">
-        <v>276</v>
+        <v>239</v>
       </c>
       <c r="D43" t="s">
-        <v>279</v>
+        <v>242</v>
       </c>
       <c r="E43" t="s">
-        <v>280</v>
+        <v>243</v>
       </c>
       <c r="F43" t="s">
         <v>12</v>
@@ -2797,21 +2791,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>78</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>127</v>
+    <row r="44" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>97</v>
       </c>
       <c r="C44" t="s">
-        <v>239</v>
+        <v>208</v>
       </c>
       <c r="D44" t="s">
-        <v>282</v>
+        <v>245</v>
       </c>
       <c r="E44" t="s">
-        <v>283</v>
+        <v>246</v>
       </c>
       <c r="F44" t="s">
         <v>12</v>
@@ -2821,20 +2815,20 @@
       </c>
     </row>
     <row r="45" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>232</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>233</v>
+      <c r="A45" s="6" t="s">
+        <v>417</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="C45" t="s">
-        <v>234</v>
+        <v>203</v>
       </c>
       <c r="D45" t="s">
-        <v>282</v>
+        <v>245</v>
       </c>
       <c r="E45" t="s">
-        <v>283</v>
+        <v>246</v>
       </c>
       <c r="F45" t="s">
         <v>12</v>
@@ -2844,20 +2838,20 @@
       </c>
     </row>
     <row r="46" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>254</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>128</v>
+      <c r="A46" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>98</v>
       </c>
       <c r="C46" t="s">
-        <v>240</v>
+        <v>209</v>
       </c>
       <c r="D46" t="s">
-        <v>282</v>
+        <v>245</v>
       </c>
       <c r="E46" t="s">
-        <v>283</v>
+        <v>246</v>
       </c>
       <c r="F46" t="s">
         <v>12</v>
@@ -2867,20 +2861,20 @@
       </c>
     </row>
     <row r="47" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>242</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>133</v>
+      <c r="A47" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>103</v>
       </c>
       <c r="C47" t="s">
-        <v>243</v>
+        <v>212</v>
       </c>
       <c r="D47" t="s">
-        <v>282</v>
+        <v>245</v>
       </c>
       <c r="E47" t="s">
-        <v>283</v>
+        <v>246</v>
       </c>
       <c r="F47" t="s">
         <v>12</v>
@@ -2890,20 +2884,20 @@
       </c>
     </row>
     <row r="48" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>131</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>130</v>
+      <c r="A48" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>100</v>
       </c>
       <c r="C48" t="s">
-        <v>199</v>
+        <v>169</v>
       </c>
       <c r="D48" t="s">
-        <v>282</v>
+        <v>245</v>
       </c>
       <c r="E48" t="s">
-        <v>283</v>
+        <v>246</v>
       </c>
       <c r="F48" t="s">
         <v>12</v>
@@ -2913,20 +2907,20 @@
       </c>
     </row>
     <row r="49" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>241</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>134</v>
+      <c r="A49" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>104</v>
       </c>
       <c r="C49" t="s">
-        <v>244</v>
+        <v>213</v>
       </c>
       <c r="D49" t="s">
-        <v>282</v>
+        <v>245</v>
       </c>
       <c r="E49" t="s">
-        <v>283</v>
+        <v>246</v>
       </c>
       <c r="F49" t="s">
         <v>12</v>
@@ -2936,20 +2930,20 @@
       </c>
     </row>
     <row r="50" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>62</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>108</v>
+      <c r="A50" s="6" t="s">
+        <v>419</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>78</v>
       </c>
       <c r="C50" t="s">
-        <v>182</v>
+        <v>152</v>
       </c>
       <c r="D50" t="s">
-        <v>282</v>
+        <v>245</v>
       </c>
       <c r="E50" t="s">
-        <v>283</v>
+        <v>246</v>
       </c>
       <c r="F50" t="s">
         <v>12</v>
@@ -2959,20 +2953,20 @@
       </c>
     </row>
     <row r="51" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>73</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>122</v>
+      <c r="A51" s="6" t="s">
+        <v>420</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="C51" t="s">
-        <v>197</v>
+        <v>167</v>
       </c>
       <c r="D51" t="s">
-        <v>282</v>
+        <v>245</v>
       </c>
       <c r="E51" t="s">
-        <v>283</v>
+        <v>246</v>
       </c>
       <c r="F51" t="s">
         <v>12</v>
@@ -2981,21 +2975,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>76</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>125</v>
+    <row r="52" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="C52" t="s">
-        <v>238</v>
+        <v>207</v>
       </c>
       <c r="D52" t="s">
-        <v>282</v>
+        <v>245</v>
       </c>
       <c r="E52" t="s">
-        <v>283</v>
+        <v>246</v>
       </c>
       <c r="F52" t="s">
         <v>12</v>
@@ -3005,20 +2999,20 @@
       </c>
     </row>
     <row r="53" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>77</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>126</v>
+      <c r="A53" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>96</v>
       </c>
       <c r="C53" t="s">
-        <v>202</v>
+        <v>172</v>
       </c>
       <c r="D53" t="s">
-        <v>282</v>
+        <v>245</v>
       </c>
       <c r="E53" t="s">
-        <v>283</v>
+        <v>246</v>
       </c>
       <c r="F53" t="s">
         <v>12</v>
@@ -3028,20 +3022,20 @@
       </c>
     </row>
     <row r="54" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>75</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>75</v>
+      <c r="A54" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="C54" t="s">
-        <v>200</v>
+        <v>170</v>
       </c>
       <c r="D54" t="s">
-        <v>290</v>
+        <v>253</v>
       </c>
       <c r="E54" t="s">
-        <v>291</v>
+        <v>254</v>
       </c>
       <c r="F54" t="s">
         <v>12</v>
@@ -3051,20 +3045,20 @@
       </c>
     </row>
     <row r="55" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="A55" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B55" s="2" t="s">
-        <v>124</v>
+      <c r="B55" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="C55" t="s">
-        <v>201</v>
+        <v>171</v>
       </c>
       <c r="D55" t="s">
-        <v>290</v>
+        <v>253</v>
       </c>
       <c r="E55" t="s">
-        <v>291</v>
+        <v>254</v>
       </c>
       <c r="F55" t="s">
         <v>12</v>
@@ -3074,20 +3068,20 @@
       </c>
     </row>
     <row r="56" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>81</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>135</v>
+      <c r="A56" s="6" t="s">
+        <v>421</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="C56" t="s">
-        <v>205</v>
+        <v>175</v>
       </c>
       <c r="D56" t="s">
-        <v>290</v>
+        <v>253</v>
       </c>
       <c r="E56" t="s">
-        <v>291</v>
+        <v>254</v>
       </c>
       <c r="F56" t="s">
         <v>12</v>
@@ -3097,20 +3091,20 @@
       </c>
     </row>
     <row r="57" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>235</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>236</v>
+      <c r="A57" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>205</v>
       </c>
       <c r="C57" t="s">
-        <v>237</v>
+        <v>206</v>
       </c>
       <c r="D57" t="s">
-        <v>290</v>
+        <v>253</v>
       </c>
       <c r="E57" t="s">
-        <v>291</v>
+        <v>254</v>
       </c>
       <c r="F57" t="s">
         <v>12</v>
@@ -3120,20 +3114,20 @@
       </c>
     </row>
     <row r="58" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>80</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>132</v>
+      <c r="A58" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>102</v>
       </c>
       <c r="C58" t="s">
-        <v>204</v>
+        <v>174</v>
       </c>
       <c r="D58" t="s">
-        <v>290</v>
+        <v>253</v>
       </c>
       <c r="E58" t="s">
-        <v>291</v>
+        <v>254</v>
       </c>
       <c r="F58" t="s">
         <v>12</v>
@@ -3143,20 +3137,20 @@
       </c>
     </row>
     <row r="59" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>284</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>286</v>
+      <c r="A59" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>249</v>
       </c>
       <c r="C59" t="s">
-        <v>287</v>
+        <v>250</v>
       </c>
       <c r="D59" t="s">
-        <v>290</v>
+        <v>253</v>
       </c>
       <c r="E59" t="s">
-        <v>291</v>
+        <v>254</v>
       </c>
       <c r="F59" t="s">
         <v>12</v>
@@ -3165,21 +3159,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>79</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>129</v>
+    <row r="60" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>99</v>
       </c>
       <c r="C60" t="s">
-        <v>203</v>
+        <v>173</v>
       </c>
       <c r="D60" t="s">
-        <v>290</v>
+        <v>253</v>
       </c>
       <c r="E60" t="s">
-        <v>291</v>
+        <v>254</v>
       </c>
       <c r="F60" t="s">
         <v>12</v>
@@ -3189,20 +3183,20 @@
       </c>
     </row>
     <row r="61" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>285</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>289</v>
+      <c r="A61" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>252</v>
       </c>
       <c r="C61" t="s">
-        <v>288</v>
+        <v>251</v>
       </c>
       <c r="D61" t="s">
-        <v>290</v>
+        <v>253</v>
       </c>
       <c r="E61" t="s">
-        <v>291</v>
+        <v>254</v>
       </c>
       <c r="F61" t="s">
         <v>12</v>
@@ -3212,20 +3206,20 @@
       </c>
     </row>
     <row r="62" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>74</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>123</v>
+      <c r="A62" s="6" t="s">
+        <v>422</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="C62" t="s">
-        <v>198</v>
+        <v>168</v>
       </c>
       <c r="D62" t="s">
-        <v>290</v>
+        <v>253</v>
       </c>
       <c r="E62" t="s">
-        <v>291</v>
+        <v>254</v>
       </c>
       <c r="F62" t="s">
         <v>12</v>
@@ -3235,20 +3229,20 @@
       </c>
     </row>
     <row r="63" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>86</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>140</v>
+      <c r="A63" s="6" t="s">
+        <v>423</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>110</v>
       </c>
       <c r="C63" t="s">
-        <v>209</v>
+        <v>179</v>
       </c>
       <c r="D63" t="s">
-        <v>304</v>
+        <v>263</v>
       </c>
       <c r="E63" t="s">
-        <v>305</v>
+        <v>264</v>
       </c>
       <c r="F63" t="s">
         <v>12</v>
@@ -3258,20 +3252,20 @@
       </c>
     </row>
     <row r="64" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>87</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>141</v>
+      <c r="A64" s="6" t="s">
+        <v>424</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>111</v>
       </c>
       <c r="C64" t="s">
-        <v>210</v>
+        <v>180</v>
       </c>
       <c r="D64" t="s">
-        <v>304</v>
+        <v>263</v>
       </c>
       <c r="E64" t="s">
-        <v>305</v>
+        <v>264</v>
       </c>
       <c r="F64" t="s">
         <v>12</v>
@@ -3281,20 +3275,20 @@
       </c>
     </row>
     <row r="65" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>88</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>142</v>
+      <c r="A65" s="6" t="s">
+        <v>425</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>112</v>
       </c>
       <c r="C65" t="s">
-        <v>211</v>
+        <v>181</v>
       </c>
       <c r="D65" t="s">
-        <v>304</v>
+        <v>263</v>
       </c>
       <c r="E65" t="s">
-        <v>305</v>
+        <v>264</v>
       </c>
       <c r="F65" t="s">
         <v>12</v>
@@ -3304,20 +3298,20 @@
       </c>
     </row>
     <row r="66" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>89</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>143</v>
+      <c r="A66" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>113</v>
       </c>
       <c r="C66" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="D66" t="s">
-        <v>304</v>
+        <v>263</v>
       </c>
       <c r="E66" t="s">
-        <v>305</v>
+        <v>264</v>
       </c>
       <c r="F66" t="s">
         <v>12</v>
@@ -3327,20 +3321,20 @@
       </c>
     </row>
     <row r="67" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>19</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>19</v>
+      <c r="A67" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="C67" t="s">
-        <v>213</v>
+        <v>183</v>
       </c>
       <c r="D67" t="s">
-        <v>304</v>
+        <v>263</v>
       </c>
       <c r="E67" t="s">
-        <v>305</v>
+        <v>264</v>
       </c>
       <c r="F67" t="s">
         <v>12</v>
@@ -3350,20 +3344,20 @@
       </c>
     </row>
     <row r="68" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>20</v>
-      </c>
-      <c r="B68" s="4" t="s">
-        <v>20</v>
+      <c r="A68" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="C68" t="s">
-        <v>214</v>
+        <v>184</v>
       </c>
       <c r="D68" t="s">
-        <v>304</v>
+        <v>263</v>
       </c>
       <c r="E68" t="s">
-        <v>305</v>
+        <v>264</v>
       </c>
       <c r="F68" t="s">
         <v>12</v>
@@ -3373,20 +3367,20 @@
       </c>
     </row>
     <row r="69" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>98</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>98</v>
+      <c r="A69" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="C69" t="s">
-        <v>215</v>
+        <v>185</v>
       </c>
       <c r="D69" t="s">
-        <v>304</v>
+        <v>263</v>
       </c>
       <c r="E69" t="s">
-        <v>305</v>
+        <v>264</v>
       </c>
       <c r="F69" t="s">
         <v>12</v>
@@ -3396,20 +3390,20 @@
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>292</v>
+      <c r="A70" s="6" t="s">
+        <v>426</v>
       </c>
       <c r="B70" t="s">
-        <v>296</v>
+        <v>255</v>
       </c>
       <c r="C70" t="s">
-        <v>297</v>
+        <v>256</v>
       </c>
       <c r="D70" t="s">
-        <v>304</v>
+        <v>263</v>
       </c>
       <c r="E70" t="s">
-        <v>305</v>
+        <v>264</v>
       </c>
       <c r="F70" t="s">
         <v>12</v>
@@ -3419,20 +3413,20 @@
       </c>
     </row>
     <row r="71" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>23</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>146</v>
+      <c r="A71" s="6" t="s">
+        <v>427</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>116</v>
       </c>
       <c r="C71" t="s">
-        <v>217</v>
+        <v>187</v>
       </c>
       <c r="D71" t="s">
-        <v>304</v>
+        <v>263</v>
       </c>
       <c r="E71" t="s">
-        <v>305</v>
+        <v>264</v>
       </c>
       <c r="F71" t="s">
         <v>12</v>
@@ -3442,20 +3436,20 @@
       </c>
     </row>
     <row r="72" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>293</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>301</v>
+      <c r="A72" s="6" t="s">
+        <v>428</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>260</v>
       </c>
       <c r="C72" t="s">
-        <v>298</v>
+        <v>257</v>
       </c>
       <c r="D72" t="s">
-        <v>304</v>
+        <v>263</v>
       </c>
       <c r="E72" t="s">
-        <v>305</v>
+        <v>264</v>
       </c>
       <c r="F72" t="s">
         <v>12</v>
@@ -3465,20 +3459,20 @@
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>294</v>
-      </c>
-      <c r="B73" s="6" t="s">
-        <v>302</v>
+      <c r="A73" s="6" t="s">
+        <v>429</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>261</v>
       </c>
       <c r="C73" t="s">
-        <v>299</v>
+        <v>258</v>
       </c>
       <c r="D73" t="s">
-        <v>304</v>
+        <v>263</v>
       </c>
       <c r="E73" t="s">
-        <v>305</v>
+        <v>264</v>
       </c>
       <c r="F73" t="s">
         <v>12</v>
@@ -3488,20 +3482,20 @@
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>295</v>
-      </c>
-      <c r="B74" s="6" t="s">
-        <v>303</v>
+      <c r="A74" s="6" t="s">
+        <v>430</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>262</v>
       </c>
       <c r="C74" t="s">
-        <v>300</v>
+        <v>259</v>
       </c>
       <c r="D74" t="s">
-        <v>304</v>
+        <v>263</v>
       </c>
       <c r="E74" t="s">
-        <v>305</v>
+        <v>264</v>
       </c>
       <c r="F74" t="s">
         <v>12</v>
@@ -3511,20 +3505,20 @@
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>306</v>
+      <c r="A75" s="6" t="s">
+        <v>265</v>
       </c>
       <c r="B75" t="s">
-        <v>308</v>
+        <v>267</v>
       </c>
       <c r="C75" t="s">
-        <v>311</v>
+        <v>270</v>
       </c>
       <c r="D75" t="s">
-        <v>313</v>
+        <v>272</v>
       </c>
       <c r="E75" t="s">
-        <v>314</v>
+        <v>273</v>
       </c>
       <c r="F75" t="s">
         <v>12</v>
@@ -3534,20 +3528,20 @@
       </c>
     </row>
     <row r="76" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>65</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>111</v>
+      <c r="A76" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="C76" t="s">
-        <v>184</v>
+        <v>154</v>
       </c>
       <c r="D76" t="s">
-        <v>313</v>
+        <v>272</v>
       </c>
       <c r="E76" t="s">
-        <v>314</v>
+        <v>273</v>
       </c>
       <c r="F76" t="s">
         <v>12</v>
@@ -3557,20 +3551,20 @@
       </c>
     </row>
     <row r="77" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>64</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>110</v>
+      <c r="A77" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>80</v>
       </c>
       <c r="C77" t="s">
-        <v>183</v>
+        <v>153</v>
       </c>
       <c r="D77" t="s">
-        <v>313</v>
+        <v>272</v>
       </c>
       <c r="E77" t="s">
-        <v>314</v>
+        <v>273</v>
       </c>
       <c r="F77" t="s">
         <v>12</v>
@@ -3580,20 +3574,20 @@
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>307</v>
+      <c r="A78" s="6" t="s">
+        <v>266</v>
       </c>
       <c r="B78" t="s">
-        <v>309</v>
+        <v>268</v>
       </c>
       <c r="C78" t="s">
-        <v>312</v>
+        <v>271</v>
       </c>
       <c r="D78" t="s">
-        <v>313</v>
+        <v>272</v>
       </c>
       <c r="E78" t="s">
-        <v>314</v>
+        <v>273</v>
       </c>
       <c r="F78" t="s">
         <v>12</v>
@@ -3603,20 +3597,20 @@
       </c>
     </row>
     <row r="79" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>57</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>103</v>
+      <c r="A79" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="C79" t="s">
-        <v>177</v>
+        <v>147</v>
       </c>
       <c r="D79" t="s">
-        <v>313</v>
+        <v>272</v>
       </c>
       <c r="E79" t="s">
-        <v>314</v>
+        <v>273</v>
       </c>
       <c r="F79" t="s">
         <v>12</v>
@@ -3626,20 +3620,20 @@
       </c>
     </row>
     <row r="80" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>90</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>144</v>
+      <c r="A80" s="6" t="s">
+        <v>431</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>114</v>
       </c>
       <c r="C80" t="s">
-        <v>216</v>
+        <v>186</v>
       </c>
       <c r="D80" t="s">
-        <v>313</v>
+        <v>272</v>
       </c>
       <c r="E80" t="s">
-        <v>314</v>
+        <v>273</v>
       </c>
       <c r="F80" t="s">
         <v>12</v>
@@ -3649,20 +3643,20 @@
       </c>
     </row>
     <row r="81" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>58</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>104</v>
+      <c r="A81" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="C81" t="s">
-        <v>178</v>
+        <v>148</v>
       </c>
       <c r="D81" t="s">
-        <v>313</v>
+        <v>272</v>
       </c>
       <c r="E81" t="s">
-        <v>314</v>
+        <v>273</v>
       </c>
       <c r="F81" t="s">
         <v>12</v>
@@ -3672,20 +3666,20 @@
       </c>
     </row>
     <row r="82" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>61</v>
-      </c>
-      <c r="B82" s="4" t="s">
-        <v>107</v>
+      <c r="A82" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>77</v>
       </c>
       <c r="C82" t="s">
-        <v>181</v>
+        <v>151</v>
       </c>
       <c r="D82" t="s">
-        <v>313</v>
+        <v>272</v>
       </c>
       <c r="E82" t="s">
-        <v>314</v>
+        <v>273</v>
       </c>
       <c r="F82" t="s">
         <v>12</v>
@@ -3694,21 +3688,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>101</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>159</v>
+    <row r="83" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A83" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>129</v>
       </c>
       <c r="C83" t="s">
-        <v>229</v>
+        <v>199</v>
       </c>
       <c r="D83" t="s">
-        <v>313</v>
+        <v>272</v>
       </c>
       <c r="E83" t="s">
-        <v>314</v>
+        <v>273</v>
       </c>
       <c r="F83" t="s">
         <v>12</v>
@@ -3717,21 +3711,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>252</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>310</v>
+    <row r="84" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A84" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>269</v>
       </c>
       <c r="C84" t="s">
-        <v>190</v>
+        <v>160</v>
       </c>
       <c r="D84" t="s">
-        <v>313</v>
+        <v>272</v>
       </c>
       <c r="E84" t="s">
-        <v>314</v>
+        <v>273</v>
       </c>
       <c r="F84" t="s">
         <v>12</v>
@@ -3741,20 +3735,20 @@
       </c>
     </row>
     <row r="85" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>100</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>151</v>
+      <c r="A85" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>121</v>
       </c>
       <c r="C85" t="s">
-        <v>222</v>
+        <v>192</v>
       </c>
       <c r="D85" t="s">
-        <v>318</v>
+        <v>277</v>
       </c>
       <c r="E85" t="s">
-        <v>323</v>
+        <v>282</v>
       </c>
       <c r="F85" t="s">
         <v>12</v>
@@ -3764,20 +3758,20 @@
       </c>
     </row>
     <row r="86" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>315</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>317</v>
+      <c r="A86" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>276</v>
       </c>
       <c r="C86" t="s">
-        <v>316</v>
+        <v>275</v>
       </c>
       <c r="D86" t="s">
-        <v>318</v>
+        <v>277</v>
       </c>
       <c r="E86" t="s">
-        <v>323</v>
+        <v>282</v>
       </c>
       <c r="F86" t="s">
         <v>12</v>
@@ -3786,21 +3780,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>93</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>150</v>
+    <row r="87" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A87" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>120</v>
       </c>
       <c r="C87" t="s">
-        <v>221</v>
+        <v>191</v>
       </c>
       <c r="D87" t="s">
-        <v>318</v>
+        <v>277</v>
       </c>
       <c r="E87" t="s">
-        <v>323</v>
+        <v>282</v>
       </c>
       <c r="F87" t="s">
         <v>12</v>
@@ -3810,20 +3804,20 @@
       </c>
     </row>
     <row r="88" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>17</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>153</v>
+      <c r="A88" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="C88" t="s">
-        <v>224</v>
+        <v>194</v>
       </c>
       <c r="D88" t="s">
-        <v>318</v>
+        <v>277</v>
       </c>
       <c r="E88" t="s">
-        <v>323</v>
+        <v>282</v>
       </c>
       <c r="F88" t="s">
         <v>12</v>
@@ -3833,20 +3827,20 @@
       </c>
     </row>
     <row r="89" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>91</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>147</v>
+      <c r="A89" s="6" t="s">
+        <v>432</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>117</v>
       </c>
       <c r="C89" t="s">
-        <v>218</v>
+        <v>188</v>
       </c>
       <c r="D89" t="s">
-        <v>318</v>
+        <v>277</v>
       </c>
       <c r="E89" t="s">
-        <v>323</v>
+        <v>282</v>
       </c>
       <c r="F89" t="s">
         <v>12</v>
@@ -3856,20 +3850,20 @@
       </c>
     </row>
     <row r="90" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>247</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>246</v>
+      <c r="A90" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>215</v>
       </c>
       <c r="C90" t="s">
-        <v>245</v>
+        <v>214</v>
       </c>
       <c r="D90" t="s">
-        <v>318</v>
+        <v>277</v>
       </c>
       <c r="E90" t="s">
-        <v>323</v>
+        <v>282</v>
       </c>
       <c r="F90" t="s">
         <v>12</v>
@@ -3879,20 +3873,20 @@
       </c>
     </row>
     <row r="91" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>24</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>154</v>
+      <c r="A91" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>124</v>
       </c>
       <c r="C91" t="s">
-        <v>225</v>
+        <v>195</v>
       </c>
       <c r="D91" t="s">
-        <v>318</v>
+        <v>277</v>
       </c>
       <c r="E91" t="s">
-        <v>323</v>
+        <v>282</v>
       </c>
       <c r="F91" t="s">
         <v>12</v>
@@ -3902,20 +3896,20 @@
       </c>
     </row>
     <row r="92" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>94</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>155</v>
+      <c r="A92" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>125</v>
       </c>
       <c r="C92" t="s">
-        <v>248</v>
+        <v>217</v>
       </c>
       <c r="D92" t="s">
-        <v>322</v>
+        <v>281</v>
       </c>
       <c r="E92" t="s">
-        <v>324</v>
+        <v>283</v>
       </c>
       <c r="F92" t="s">
         <v>12</v>
@@ -3925,20 +3919,20 @@
       </c>
     </row>
     <row r="93" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>138</v>
+      <c r="A93" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>108</v>
       </c>
       <c r="C93" t="s">
-        <v>208</v>
+        <v>178</v>
       </c>
       <c r="D93" t="s">
-        <v>322</v>
+        <v>281</v>
       </c>
       <c r="E93" t="s">
-        <v>324</v>
+        <v>283</v>
       </c>
       <c r="F93" t="s">
         <v>12</v>
@@ -3948,20 +3942,20 @@
       </c>
     </row>
     <row r="94" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>95</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>156</v>
+      <c r="A94" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>126</v>
       </c>
       <c r="C94" t="s">
-        <v>226</v>
+        <v>196</v>
       </c>
       <c r="D94" t="s">
-        <v>322</v>
+        <v>281</v>
       </c>
       <c r="E94" t="s">
-        <v>324</v>
+        <v>283</v>
       </c>
       <c r="F94" t="s">
         <v>12</v>
@@ -3971,20 +3965,20 @@
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>319</v>
-      </c>
-      <c r="B95" s="6" t="s">
-        <v>320</v>
+      <c r="A95" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="B95" s="5" t="s">
+        <v>279</v>
       </c>
       <c r="C95" t="s">
-        <v>321</v>
+        <v>280</v>
       </c>
       <c r="D95" t="s">
-        <v>322</v>
+        <v>281</v>
       </c>
       <c r="E95" t="s">
-        <v>324</v>
+        <v>283</v>
       </c>
       <c r="F95" t="s">
         <v>12</v>
@@ -3994,20 +3988,20 @@
       </c>
     </row>
     <row r="96" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>96</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>157</v>
+      <c r="A96" s="6" t="s">
+        <v>434</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>127</v>
       </c>
       <c r="C96" t="s">
-        <v>227</v>
+        <v>197</v>
       </c>
       <c r="D96" t="s">
-        <v>335</v>
+        <v>292</v>
       </c>
       <c r="E96" t="s">
-        <v>336</v>
+        <v>293</v>
       </c>
       <c r="F96" t="s">
         <v>12</v>
@@ -4017,20 +4011,20 @@
       </c>
     </row>
     <row r="97" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>325</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>25</v>
+      <c r="A97" s="6" t="s">
+        <v>435</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="C97" t="s">
-        <v>255</v>
+        <v>221</v>
       </c>
       <c r="D97" t="s">
-        <v>335</v>
+        <v>292</v>
       </c>
       <c r="E97" t="s">
-        <v>336</v>
+        <v>293</v>
       </c>
       <c r="F97" t="s">
         <v>12</v>
@@ -4040,20 +4034,20 @@
       </c>
     </row>
     <row r="98" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>83</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>137</v>
+      <c r="A98" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="C98" t="s">
-        <v>207</v>
+        <v>177</v>
       </c>
       <c r="D98" t="s">
-        <v>335</v>
+        <v>292</v>
       </c>
       <c r="E98" t="s">
-        <v>336</v>
+        <v>293</v>
       </c>
       <c r="F98" t="s">
         <v>12</v>
@@ -4063,20 +4057,20 @@
       </c>
     </row>
     <row r="99" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>92</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>148</v>
+      <c r="A99" s="6" t="s">
+        <v>436</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>118</v>
       </c>
       <c r="C99" t="s">
-        <v>219</v>
+        <v>189</v>
       </c>
       <c r="D99" t="s">
-        <v>335</v>
+        <v>292</v>
       </c>
       <c r="E99" t="s">
-        <v>336</v>
+        <v>293</v>
       </c>
       <c r="F99" t="s">
         <v>12</v>
@@ -4086,20 +4080,20 @@
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>326</v>
+      <c r="A100" s="6" t="s">
+        <v>284</v>
       </c>
       <c r="B100" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="C100" t="s">
-        <v>333</v>
+        <v>290</v>
       </c>
       <c r="D100" t="s">
-        <v>335</v>
+        <v>292</v>
       </c>
       <c r="E100" t="s">
-        <v>336</v>
+        <v>293</v>
       </c>
       <c r="F100" t="s">
         <v>12</v>
@@ -4109,20 +4103,20 @@
       </c>
     </row>
     <row r="101" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>99</v>
-      </c>
-      <c r="B101" s="4" t="s">
-        <v>149</v>
+      <c r="A101" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>119</v>
       </c>
       <c r="C101" t="s">
-        <v>220</v>
+        <v>190</v>
       </c>
       <c r="D101" t="s">
-        <v>335</v>
+        <v>292</v>
       </c>
       <c r="E101" t="s">
-        <v>336</v>
+        <v>293</v>
       </c>
       <c r="F101" t="s">
         <v>12</v>
@@ -4132,20 +4126,20 @@
       </c>
     </row>
     <row r="102" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>327</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>330</v>
+      <c r="A102" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>287</v>
       </c>
       <c r="C102" t="s">
-        <v>332</v>
+        <v>289</v>
       </c>
       <c r="D102" t="s">
-        <v>335</v>
+        <v>292</v>
       </c>
       <c r="E102" t="s">
-        <v>336</v>
+        <v>293</v>
       </c>
       <c r="F102" t="s">
         <v>12</v>
@@ -4155,20 +4149,20 @@
       </c>
     </row>
     <row r="103" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>69</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>118</v>
+      <c r="A103" s="6" t="s">
+        <v>437</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="C103" t="s">
-        <v>192</v>
+        <v>162</v>
       </c>
       <c r="D103" t="s">
-        <v>335</v>
+        <v>292</v>
       </c>
       <c r="E103" t="s">
-        <v>336</v>
+        <v>293</v>
       </c>
       <c r="F103" t="s">
         <v>12</v>
@@ -4178,20 +4172,20 @@
       </c>
     </row>
     <row r="104" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>21</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>152</v>
+      <c r="A104" s="6" t="s">
+        <v>438</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>122</v>
       </c>
       <c r="C104" t="s">
-        <v>223</v>
+        <v>193</v>
       </c>
       <c r="D104" t="s">
-        <v>335</v>
+        <v>292</v>
       </c>
       <c r="E104" t="s">
-        <v>336</v>
+        <v>293</v>
       </c>
       <c r="F104" t="s">
         <v>12</v>
@@ -4201,20 +4195,20 @@
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>328</v>
-      </c>
-      <c r="B105" s="6" t="s">
-        <v>331</v>
+      <c r="A105" s="6" t="s">
+        <v>439</v>
+      </c>
+      <c r="B105" s="5" t="s">
+        <v>288</v>
       </c>
       <c r="C105" t="s">
-        <v>334</v>
+        <v>291</v>
       </c>
       <c r="D105" t="s">
-        <v>335</v>
+        <v>292</v>
       </c>
       <c r="E105" t="s">
-        <v>336</v>
+        <v>293</v>
       </c>
       <c r="F105" t="s">
         <v>12</v>
@@ -4224,20 +4218,20 @@
       </c>
     </row>
     <row r="106" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>253</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>145</v>
+      <c r="A106" s="6" t="s">
+        <v>440</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>115</v>
       </c>
       <c r="C106" t="s">
-        <v>249</v>
+        <v>218</v>
       </c>
       <c r="D106" t="s">
-        <v>335</v>
+        <v>292</v>
       </c>
       <c r="E106" t="s">
-        <v>336</v>
+        <v>293</v>
       </c>
       <c r="F106" t="s">
         <v>12</v>
@@ -4248,19 +4242,19 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B107" t="s">
+        <v>22</v>
+      </c>
+      <c r="C107" t="s">
         <v>27</v>
       </c>
-      <c r="C107" t="s">
-        <v>32</v>
-      </c>
       <c r="D107" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E107" t="s">
-        <v>386</v>
+        <v>340</v>
       </c>
       <c r="F107" t="s">
         <v>12</v>
@@ -4271,19 +4265,19 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B108" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C108" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D108" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E108" t="s">
-        <v>386</v>
+        <v>340</v>
       </c>
       <c r="F108" t="s">
         <v>12</v>
@@ -4294,13 +4288,13 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C109" t="s">
-        <v>346</v>
+        <v>300</v>
       </c>
       <c r="D109" t="s">
-        <v>385</v>
+        <v>339</v>
       </c>
       <c r="E109" t="s">
-        <v>387</v>
+        <v>341</v>
       </c>
       <c r="F109" t="s">
         <v>12</v>
@@ -4311,13 +4305,13 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C110" t="s">
-        <v>347</v>
+        <v>301</v>
       </c>
       <c r="D110" t="s">
-        <v>385</v>
+        <v>339</v>
       </c>
       <c r="E110" t="s">
-        <v>387</v>
+        <v>341</v>
       </c>
       <c r="F110" t="s">
         <v>12</v>
@@ -4328,13 +4322,13 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C111" t="s">
-        <v>348</v>
+        <v>302</v>
       </c>
       <c r="D111" t="s">
-        <v>385</v>
+        <v>339</v>
       </c>
       <c r="E111" t="s">
-        <v>387</v>
+        <v>341</v>
       </c>
       <c r="F111" t="s">
         <v>12</v>
@@ -4345,13 +4339,13 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C112" t="s">
-        <v>349</v>
+        <v>303</v>
       </c>
       <c r="D112" t="s">
-        <v>385</v>
+        <v>339</v>
       </c>
       <c r="E112" t="s">
-        <v>387</v>
+        <v>341</v>
       </c>
       <c r="F112" t="s">
         <v>12</v>
@@ -4362,13 +4356,13 @@
     </row>
     <row r="113" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C113" t="s">
-        <v>350</v>
+        <v>304</v>
       </c>
       <c r="D113" t="s">
-        <v>385</v>
+        <v>339</v>
       </c>
       <c r="E113" t="s">
-        <v>387</v>
+        <v>341</v>
       </c>
       <c r="F113" t="s">
         <v>12</v>
@@ -4379,13 +4373,13 @@
     </row>
     <row r="114" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C114" t="s">
-        <v>351</v>
+        <v>305</v>
       </c>
       <c r="D114" t="s">
-        <v>385</v>
+        <v>339</v>
       </c>
       <c r="E114" t="s">
-        <v>387</v>
+        <v>341</v>
       </c>
       <c r="F114" t="s">
         <v>12</v>
@@ -4396,13 +4390,13 @@
     </row>
     <row r="115" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C115" t="s">
-        <v>352</v>
+        <v>306</v>
       </c>
       <c r="D115" t="s">
-        <v>385</v>
+        <v>339</v>
       </c>
       <c r="E115" t="s">
-        <v>387</v>
+        <v>341</v>
       </c>
       <c r="F115" t="s">
         <v>12</v>
@@ -4413,13 +4407,13 @@
     </row>
     <row r="116" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C116" t="s">
-        <v>353</v>
+        <v>307</v>
       </c>
       <c r="D116" t="s">
-        <v>385</v>
+        <v>339</v>
       </c>
       <c r="E116" t="s">
-        <v>387</v>
+        <v>341</v>
       </c>
       <c r="F116" t="s">
         <v>12</v>
@@ -4430,13 +4424,13 @@
     </row>
     <row r="117" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C117" t="s">
-        <v>354</v>
+        <v>308</v>
       </c>
       <c r="D117" t="s">
-        <v>385</v>
+        <v>339</v>
       </c>
       <c r="E117" t="s">
-        <v>387</v>
+        <v>341</v>
       </c>
       <c r="F117" t="s">
         <v>12</v>
@@ -4447,13 +4441,13 @@
     </row>
     <row r="118" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C118" t="s">
-        <v>355</v>
+        <v>309</v>
       </c>
       <c r="D118" t="s">
-        <v>385</v>
+        <v>339</v>
       </c>
       <c r="E118" t="s">
-        <v>387</v>
+        <v>341</v>
       </c>
       <c r="F118" t="s">
         <v>12</v>
@@ -4464,13 +4458,13 @@
     </row>
     <row r="119" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C119" t="s">
-        <v>356</v>
+        <v>310</v>
       </c>
       <c r="D119" t="s">
-        <v>385</v>
+        <v>339</v>
       </c>
       <c r="E119" t="s">
-        <v>387</v>
+        <v>341</v>
       </c>
       <c r="F119" t="s">
         <v>12</v>
@@ -4481,13 +4475,13 @@
     </row>
     <row r="120" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C120" t="s">
-        <v>357</v>
+        <v>311</v>
       </c>
       <c r="D120" t="s">
-        <v>385</v>
+        <v>339</v>
       </c>
       <c r="E120" t="s">
-        <v>387</v>
+        <v>341</v>
       </c>
       <c r="F120" t="s">
         <v>12</v>
@@ -4498,13 +4492,13 @@
     </row>
     <row r="121" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C121" t="s">
-        <v>358</v>
+        <v>312</v>
       </c>
       <c r="D121" t="s">
-        <v>385</v>
+        <v>339</v>
       </c>
       <c r="E121" t="s">
-        <v>387</v>
+        <v>341</v>
       </c>
       <c r="F121" t="s">
         <v>12</v>
@@ -4515,13 +4509,13 @@
     </row>
     <row r="122" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C122" t="s">
-        <v>359</v>
+        <v>313</v>
       </c>
       <c r="D122" t="s">
-        <v>385</v>
+        <v>339</v>
       </c>
       <c r="E122" t="s">
-        <v>387</v>
+        <v>341</v>
       </c>
       <c r="F122" t="s">
         <v>12</v>
@@ -4532,13 +4526,13 @@
     </row>
     <row r="123" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C123" t="s">
-        <v>360</v>
+        <v>314</v>
       </c>
       <c r="D123" t="s">
-        <v>385</v>
+        <v>339</v>
       </c>
       <c r="E123" t="s">
-        <v>387</v>
+        <v>341</v>
       </c>
       <c r="F123" t="s">
         <v>12</v>
@@ -4549,13 +4543,13 @@
     </row>
     <row r="124" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C124" t="s">
-        <v>361</v>
+        <v>315</v>
       </c>
       <c r="D124" t="s">
-        <v>385</v>
+        <v>339</v>
       </c>
       <c r="E124" t="s">
-        <v>387</v>
+        <v>341</v>
       </c>
       <c r="F124" t="s">
         <v>12</v>
@@ -4566,13 +4560,13 @@
     </row>
     <row r="125" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C125" t="s">
-        <v>362</v>
+        <v>316</v>
       </c>
       <c r="D125" t="s">
-        <v>385</v>
+        <v>339</v>
       </c>
       <c r="E125" t="s">
-        <v>387</v>
+        <v>341</v>
       </c>
       <c r="F125" t="s">
         <v>12</v>
@@ -4583,13 +4577,13 @@
     </row>
     <row r="126" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C126" t="s">
-        <v>363</v>
+        <v>317</v>
       </c>
       <c r="D126" t="s">
-        <v>385</v>
+        <v>339</v>
       </c>
       <c r="E126" t="s">
-        <v>387</v>
+        <v>341</v>
       </c>
       <c r="F126" t="s">
         <v>12</v>
@@ -4600,13 +4594,13 @@
     </row>
     <row r="127" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C127" t="s">
-        <v>364</v>
+        <v>318</v>
       </c>
       <c r="D127" t="s">
-        <v>385</v>
+        <v>339</v>
       </c>
       <c r="E127" t="s">
-        <v>387</v>
+        <v>341</v>
       </c>
       <c r="F127" t="s">
         <v>12</v>
@@ -4617,13 +4611,13 @@
     </row>
     <row r="128" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C128" t="s">
-        <v>365</v>
+        <v>319</v>
       </c>
       <c r="D128" t="s">
-        <v>385</v>
+        <v>339</v>
       </c>
       <c r="E128" t="s">
-        <v>387</v>
+        <v>341</v>
       </c>
       <c r="F128" t="s">
         <v>12</v>
@@ -4634,13 +4628,13 @@
     </row>
     <row r="129" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C129" t="s">
-        <v>366</v>
+        <v>320</v>
       </c>
       <c r="D129" t="s">
-        <v>385</v>
+        <v>339</v>
       </c>
       <c r="E129" t="s">
-        <v>387</v>
+        <v>341</v>
       </c>
       <c r="F129" t="s">
         <v>12</v>
@@ -4651,13 +4645,13 @@
     </row>
     <row r="130" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C130" t="s">
-        <v>367</v>
+        <v>321</v>
       </c>
       <c r="D130" t="s">
-        <v>385</v>
+        <v>339</v>
       </c>
       <c r="E130" t="s">
-        <v>387</v>
+        <v>341</v>
       </c>
       <c r="F130" t="s">
         <v>12</v>
@@ -4668,13 +4662,13 @@
     </row>
     <row r="131" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C131" t="s">
-        <v>368</v>
+        <v>322</v>
       </c>
       <c r="D131" t="s">
-        <v>385</v>
+        <v>339</v>
       </c>
       <c r="E131" t="s">
-        <v>387</v>
+        <v>341</v>
       </c>
       <c r="F131" t="s">
         <v>12</v>
@@ -4685,13 +4679,13 @@
     </row>
     <row r="132" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C132" t="s">
-        <v>369</v>
+        <v>323</v>
       </c>
       <c r="D132" t="s">
-        <v>385</v>
+        <v>339</v>
       </c>
       <c r="E132" t="s">
-        <v>387</v>
+        <v>341</v>
       </c>
       <c r="F132" t="s">
         <v>12</v>
@@ -4702,13 +4696,13 @@
     </row>
     <row r="133" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C133" t="s">
-        <v>370</v>
+        <v>324</v>
       </c>
       <c r="D133" t="s">
-        <v>385</v>
+        <v>339</v>
       </c>
       <c r="E133" t="s">
-        <v>387</v>
+        <v>341</v>
       </c>
       <c r="F133" t="s">
         <v>12</v>
@@ -4719,13 +4713,13 @@
     </row>
     <row r="134" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C134" t="s">
-        <v>371</v>
+        <v>325</v>
       </c>
       <c r="D134" t="s">
-        <v>385</v>
+        <v>339</v>
       </c>
       <c r="E134" t="s">
-        <v>387</v>
+        <v>341</v>
       </c>
       <c r="F134" t="s">
         <v>12</v>
@@ -4736,13 +4730,13 @@
     </row>
     <row r="135" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C135" t="s">
-        <v>372</v>
+        <v>326</v>
       </c>
       <c r="D135" t="s">
-        <v>385</v>
+        <v>339</v>
       </c>
       <c r="E135" t="s">
-        <v>387</v>
+        <v>341</v>
       </c>
       <c r="F135" t="s">
         <v>12</v>
@@ -4753,13 +4747,13 @@
     </row>
     <row r="136" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C136" t="s">
-        <v>373</v>
+        <v>327</v>
       </c>
       <c r="D136" t="s">
-        <v>385</v>
+        <v>339</v>
       </c>
       <c r="E136" t="s">
-        <v>387</v>
+        <v>341</v>
       </c>
       <c r="F136" t="s">
         <v>12</v>
@@ -4770,13 +4764,13 @@
     </row>
     <row r="137" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C137" t="s">
-        <v>374</v>
+        <v>328</v>
       </c>
       <c r="D137" t="s">
-        <v>385</v>
+        <v>339</v>
       </c>
       <c r="E137" t="s">
-        <v>387</v>
+        <v>341</v>
       </c>
       <c r="F137" t="s">
         <v>12</v>
@@ -4787,13 +4781,13 @@
     </row>
     <row r="138" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C138" t="s">
-        <v>375</v>
+        <v>329</v>
       </c>
       <c r="D138" t="s">
-        <v>385</v>
+        <v>339</v>
       </c>
       <c r="E138" t="s">
-        <v>387</v>
+        <v>341</v>
       </c>
       <c r="F138" t="s">
         <v>12</v>
@@ -4804,13 +4798,13 @@
     </row>
     <row r="139" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C139" t="s">
-        <v>376</v>
+        <v>330</v>
       </c>
       <c r="D139" t="s">
-        <v>385</v>
+        <v>339</v>
       </c>
       <c r="E139" t="s">
-        <v>387</v>
+        <v>341</v>
       </c>
       <c r="F139" t="s">
         <v>12</v>
@@ -4821,13 +4815,13 @@
     </row>
     <row r="140" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C140" t="s">
-        <v>377</v>
+        <v>331</v>
       </c>
       <c r="D140" t="s">
-        <v>385</v>
+        <v>339</v>
       </c>
       <c r="E140" t="s">
-        <v>387</v>
+        <v>341</v>
       </c>
       <c r="F140" t="s">
         <v>12</v>
@@ -4838,13 +4832,13 @@
     </row>
     <row r="141" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C141" t="s">
-        <v>378</v>
+        <v>332</v>
       </c>
       <c r="D141" t="s">
-        <v>385</v>
+        <v>339</v>
       </c>
       <c r="E141" t="s">
-        <v>387</v>
+        <v>341</v>
       </c>
       <c r="F141" t="s">
         <v>12</v>
@@ -4855,13 +4849,13 @@
     </row>
     <row r="142" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C142" t="s">
-        <v>379</v>
+        <v>333</v>
       </c>
       <c r="D142" t="s">
-        <v>385</v>
+        <v>339</v>
       </c>
       <c r="E142" t="s">
-        <v>387</v>
+        <v>341</v>
       </c>
       <c r="F142" t="s">
         <v>12</v>
@@ -4872,13 +4866,13 @@
     </row>
     <row r="143" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C143" t="s">
-        <v>380</v>
+        <v>334</v>
       </c>
       <c r="D143" t="s">
-        <v>385</v>
+        <v>339</v>
       </c>
       <c r="E143" t="s">
-        <v>387</v>
+        <v>341</v>
       </c>
       <c r="F143" t="s">
         <v>12</v>
@@ -4889,13 +4883,13 @@
     </row>
     <row r="144" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C144" t="s">
-        <v>381</v>
+        <v>335</v>
       </c>
       <c r="D144" t="s">
-        <v>385</v>
+        <v>339</v>
       </c>
       <c r="E144" t="s">
-        <v>387</v>
+        <v>341</v>
       </c>
       <c r="F144" t="s">
         <v>12</v>
@@ -4906,13 +4900,13 @@
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C145" t="s">
-        <v>382</v>
+        <v>336</v>
       </c>
       <c r="D145" t="s">
-        <v>385</v>
+        <v>339</v>
       </c>
       <c r="E145" t="s">
-        <v>387</v>
+        <v>341</v>
       </c>
       <c r="F145" t="s">
         <v>12</v>
@@ -4923,13 +4917,13 @@
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C146" t="s">
-        <v>383</v>
+        <v>337</v>
       </c>
       <c r="D146" t="s">
-        <v>385</v>
+        <v>339</v>
       </c>
       <c r="E146" t="s">
-        <v>387</v>
+        <v>341</v>
       </c>
       <c r="F146" t="s">
         <v>12</v>
@@ -4940,13 +4934,13 @@
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C147" t="s">
-        <v>384</v>
+        <v>338</v>
       </c>
       <c r="D147" t="s">
-        <v>385</v>
+        <v>339</v>
       </c>
       <c r="E147" t="s">
-        <v>387</v>
+        <v>341</v>
       </c>
       <c r="F147" t="s">
         <v>12</v>
@@ -4957,13 +4951,13 @@
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C148" t="s">
-        <v>388</v>
+        <v>342</v>
       </c>
       <c r="D148" t="s">
-        <v>385</v>
+        <v>339</v>
       </c>
       <c r="E148" t="s">
-        <v>387</v>
+        <v>341</v>
       </c>
       <c r="F148" t="s">
         <v>12</v>
@@ -4974,13 +4968,13 @@
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C149" t="s">
-        <v>389</v>
+        <v>343</v>
       </c>
       <c r="D149" t="s">
-        <v>385</v>
+        <v>339</v>
       </c>
       <c r="E149" t="s">
-        <v>387</v>
+        <v>341</v>
       </c>
       <c r="F149" t="s">
         <v>12</v>
@@ -4991,13 +4985,13 @@
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C150" t="s">
-        <v>390</v>
+        <v>344</v>
       </c>
       <c r="D150" t="s">
-        <v>385</v>
+        <v>339</v>
       </c>
       <c r="E150" t="s">
-        <v>387</v>
+        <v>341</v>
       </c>
       <c r="F150" t="s">
         <v>12</v>
@@ -5008,13 +5002,13 @@
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C151" t="s">
-        <v>391</v>
+        <v>345</v>
       </c>
       <c r="D151" t="s">
-        <v>385</v>
+        <v>339</v>
       </c>
       <c r="E151" t="s">
-        <v>387</v>
+        <v>341</v>
       </c>
       <c r="F151" t="s">
         <v>12</v>
@@ -5025,13 +5019,13 @@
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C152" t="s">
-        <v>392</v>
+        <v>346</v>
       </c>
       <c r="D152" t="s">
-        <v>385</v>
+        <v>339</v>
       </c>
       <c r="E152" t="s">
-        <v>387</v>
+        <v>341</v>
       </c>
       <c r="F152" t="s">
         <v>12</v>
@@ -5042,13 +5036,13 @@
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C153" t="s">
-        <v>393</v>
+        <v>347</v>
       </c>
       <c r="D153" t="s">
-        <v>385</v>
+        <v>339</v>
       </c>
       <c r="E153" t="s">
-        <v>387</v>
+        <v>341</v>
       </c>
       <c r="F153" t="s">
         <v>12</v>
@@ -5059,13 +5053,13 @@
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C154" t="s">
-        <v>394</v>
+        <v>348</v>
       </c>
       <c r="D154" t="s">
-        <v>385</v>
+        <v>339</v>
       </c>
       <c r="E154" t="s">
-        <v>387</v>
+        <v>341</v>
       </c>
       <c r="F154" t="s">
         <v>12</v>
@@ -5076,13 +5070,13 @@
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C155" t="s">
-        <v>395</v>
+        <v>349</v>
       </c>
       <c r="D155" t="s">
-        <v>385</v>
+        <v>339</v>
       </c>
       <c r="E155" t="s">
-        <v>387</v>
+        <v>341</v>
       </c>
       <c r="F155" t="s">
         <v>12</v>
@@ -5093,13 +5087,13 @@
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C156" t="s">
-        <v>396</v>
+        <v>350</v>
       </c>
       <c r="D156" t="s">
-        <v>385</v>
+        <v>339</v>
       </c>
       <c r="E156" t="s">
-        <v>387</v>
+        <v>341</v>
       </c>
       <c r="F156" t="s">
         <v>12</v>
@@ -5113,13 +5107,13 @@
         <v>1</v>
       </c>
       <c r="C157" t="s">
-        <v>397</v>
+        <v>351</v>
       </c>
       <c r="D157" t="s">
-        <v>258</v>
+        <v>224</v>
       </c>
       <c r="E157" t="s">
-        <v>415</v>
+        <v>369</v>
       </c>
       <c r="F157" t="s">
         <v>12</v>
@@ -5133,13 +5127,13 @@
         <v>2</v>
       </c>
       <c r="C158" t="s">
-        <v>398</v>
+        <v>352</v>
       </c>
       <c r="D158" t="s">
-        <v>258</v>
+        <v>224</v>
       </c>
       <c r="E158" t="s">
-        <v>415</v>
+        <v>369</v>
       </c>
       <c r="F158" t="s">
         <v>12</v>
@@ -5153,13 +5147,13 @@
         <v>3</v>
       </c>
       <c r="C159" t="s">
-        <v>399</v>
+        <v>353</v>
       </c>
       <c r="D159" t="s">
-        <v>258</v>
+        <v>224</v>
       </c>
       <c r="E159" t="s">
-        <v>415</v>
+        <v>369</v>
       </c>
       <c r="F159" t="s">
         <v>12</v>
@@ -5173,13 +5167,13 @@
         <v>4</v>
       </c>
       <c r="C160" t="s">
-        <v>400</v>
+        <v>354</v>
       </c>
       <c r="D160" t="s">
-        <v>258</v>
+        <v>224</v>
       </c>
       <c r="E160" t="s">
-        <v>415</v>
+        <v>369</v>
       </c>
       <c r="F160" t="s">
         <v>12</v>
@@ -5193,13 +5187,13 @@
         <v>5</v>
       </c>
       <c r="C161" t="s">
-        <v>401</v>
+        <v>355</v>
       </c>
       <c r="D161" t="s">
-        <v>258</v>
+        <v>224</v>
       </c>
       <c r="E161" t="s">
-        <v>415</v>
+        <v>369</v>
       </c>
       <c r="F161" t="s">
         <v>12</v>
@@ -5213,13 +5207,13 @@
         <v>6</v>
       </c>
       <c r="C162" t="s">
-        <v>402</v>
+        <v>356</v>
       </c>
       <c r="D162" t="s">
-        <v>258</v>
+        <v>224</v>
       </c>
       <c r="E162" t="s">
-        <v>415</v>
+        <v>369</v>
       </c>
       <c r="F162" t="s">
         <v>12</v>
@@ -5233,13 +5227,13 @@
         <v>7</v>
       </c>
       <c r="C163" t="s">
-        <v>403</v>
+        <v>357</v>
       </c>
       <c r="D163" t="s">
-        <v>258</v>
+        <v>224</v>
       </c>
       <c r="E163" t="s">
-        <v>415</v>
+        <v>369</v>
       </c>
       <c r="F163" t="s">
         <v>12</v>
@@ -5253,13 +5247,13 @@
         <v>8</v>
       </c>
       <c r="C164" t="s">
-        <v>404</v>
+        <v>358</v>
       </c>
       <c r="D164" t="s">
-        <v>258</v>
+        <v>224</v>
       </c>
       <c r="E164" t="s">
-        <v>415</v>
+        <v>369</v>
       </c>
       <c r="F164" t="s">
         <v>12</v>
@@ -5273,13 +5267,13 @@
         <v>9</v>
       </c>
       <c r="C165" t="s">
-        <v>405</v>
+        <v>359</v>
       </c>
       <c r="D165" t="s">
-        <v>258</v>
+        <v>224</v>
       </c>
       <c r="E165" t="s">
-        <v>415</v>
+        <v>369</v>
       </c>
       <c r="F165" t="s">
         <v>12</v>
@@ -5293,13 +5287,13 @@
         <v>10</v>
       </c>
       <c r="C166" t="s">
-        <v>406</v>
+        <v>360</v>
       </c>
       <c r="D166" t="s">
-        <v>258</v>
+        <v>224</v>
       </c>
       <c r="E166" t="s">
-        <v>415</v>
+        <v>369</v>
       </c>
       <c r="F166" t="s">
         <v>12</v>
@@ -5313,13 +5307,13 @@
         <v>11</v>
       </c>
       <c r="C167" t="s">
-        <v>407</v>
+        <v>361</v>
       </c>
       <c r="D167" t="s">
-        <v>258</v>
+        <v>224</v>
       </c>
       <c r="E167" t="s">
-        <v>415</v>
+        <v>369</v>
       </c>
       <c r="F167" t="s">
         <v>12</v>
@@ -5333,13 +5327,13 @@
         <v>12</v>
       </c>
       <c r="C168" t="s">
-        <v>408</v>
+        <v>362</v>
       </c>
       <c r="D168" t="s">
-        <v>258</v>
+        <v>224</v>
       </c>
       <c r="E168" t="s">
-        <v>415</v>
+        <v>369</v>
       </c>
       <c r="F168" t="s">
         <v>12</v>
@@ -5353,13 +5347,13 @@
         <v>13</v>
       </c>
       <c r="C169" t="s">
-        <v>409</v>
+        <v>363</v>
       </c>
       <c r="D169" t="s">
-        <v>258</v>
+        <v>224</v>
       </c>
       <c r="E169" t="s">
-        <v>415</v>
+        <v>369</v>
       </c>
       <c r="F169" t="s">
         <v>12</v>
@@ -5373,13 +5367,13 @@
         <v>14</v>
       </c>
       <c r="C170" t="s">
-        <v>410</v>
+        <v>364</v>
       </c>
       <c r="D170" t="s">
-        <v>258</v>
+        <v>224</v>
       </c>
       <c r="E170" t="s">
-        <v>415</v>
+        <v>369</v>
       </c>
       <c r="F170" t="s">
         <v>12</v>
@@ -5393,13 +5387,13 @@
         <v>15</v>
       </c>
       <c r="C171" t="s">
-        <v>411</v>
+        <v>365</v>
       </c>
       <c r="D171" t="s">
-        <v>258</v>
+        <v>224</v>
       </c>
       <c r="E171" t="s">
-        <v>415</v>
+        <v>369</v>
       </c>
       <c r="F171" t="s">
         <v>12</v>
@@ -5413,13 +5407,13 @@
         <v>16</v>
       </c>
       <c r="C172" t="s">
-        <v>412</v>
+        <v>366</v>
       </c>
       <c r="D172" t="s">
-        <v>258</v>
+        <v>224</v>
       </c>
       <c r="E172" t="s">
-        <v>415</v>
+        <v>369</v>
       </c>
       <c r="F172" t="s">
         <v>12</v>
@@ -5433,13 +5427,13 @@
         <v>17</v>
       </c>
       <c r="C173" t="s">
-        <v>413</v>
+        <v>367</v>
       </c>
       <c r="D173" t="s">
-        <v>258</v>
+        <v>224</v>
       </c>
       <c r="E173" t="s">
-        <v>415</v>
+        <v>369</v>
       </c>
       <c r="F173" t="s">
         <v>12</v>
@@ -5453,13 +5447,13 @@
         <v>18</v>
       </c>
       <c r="C174" t="s">
-        <v>429</v>
+        <v>383</v>
       </c>
       <c r="D174" t="s">
-        <v>258</v>
+        <v>224</v>
       </c>
       <c r="E174" t="s">
-        <v>415</v>
+        <v>369</v>
       </c>
       <c r="F174" t="s">
         <v>12</v>
@@ -5473,13 +5467,13 @@
         <v>19</v>
       </c>
       <c r="C175" t="s">
-        <v>430</v>
+        <v>384</v>
       </c>
       <c r="D175" t="s">
-        <v>258</v>
+        <v>224</v>
       </c>
       <c r="E175" t="s">
-        <v>415</v>
+        <v>369</v>
       </c>
       <c r="F175" t="s">
         <v>12</v>
@@ -5493,13 +5487,13 @@
         <v>20</v>
       </c>
       <c r="C176" t="s">
-        <v>431</v>
+        <v>385</v>
       </c>
       <c r="D176" t="s">
-        <v>258</v>
+        <v>224</v>
       </c>
       <c r="E176" t="s">
-        <v>415</v>
+        <v>369</v>
       </c>
       <c r="F176" t="s">
         <v>12</v>
@@ -5513,13 +5507,13 @@
         <v>21</v>
       </c>
       <c r="C177" t="s">
-        <v>432</v>
+        <v>386</v>
       </c>
       <c r="D177" t="s">
-        <v>258</v>
+        <v>224</v>
       </c>
       <c r="E177" t="s">
-        <v>415</v>
+        <v>369</v>
       </c>
       <c r="F177" t="s">
         <v>12</v>
@@ -5533,13 +5527,13 @@
         <v>22</v>
       </c>
       <c r="C178" t="s">
-        <v>433</v>
+        <v>387</v>
       </c>
       <c r="D178" t="s">
-        <v>258</v>
+        <v>224</v>
       </c>
       <c r="E178" t="s">
-        <v>415</v>
+        <v>369</v>
       </c>
       <c r="F178" t="s">
         <v>12</v>
@@ -5553,13 +5547,13 @@
         <v>23</v>
       </c>
       <c r="C179" t="s">
-        <v>434</v>
+        <v>388</v>
       </c>
       <c r="D179" t="s">
-        <v>258</v>
+        <v>224</v>
       </c>
       <c r="E179" t="s">
-        <v>415</v>
+        <v>369</v>
       </c>
       <c r="F179" t="s">
         <v>12</v>
@@ -5573,13 +5567,13 @@
         <v>24</v>
       </c>
       <c r="C180" t="s">
-        <v>435</v>
+        <v>389</v>
       </c>
       <c r="D180" t="s">
-        <v>258</v>
+        <v>224</v>
       </c>
       <c r="E180" t="s">
-        <v>415</v>
+        <v>369</v>
       </c>
       <c r="F180" t="s">
         <v>12</v>
@@ -5593,13 +5587,13 @@
         <v>25</v>
       </c>
       <c r="C181" t="s">
-        <v>436</v>
+        <v>390</v>
       </c>
       <c r="D181" t="s">
-        <v>258</v>
+        <v>224</v>
       </c>
       <c r="E181" t="s">
-        <v>415</v>
+        <v>369</v>
       </c>
       <c r="F181" t="s">
         <v>12</v>
@@ -5613,13 +5607,13 @@
         <v>26</v>
       </c>
       <c r="C182" t="s">
-        <v>437</v>
+        <v>391</v>
       </c>
       <c r="D182" t="s">
-        <v>258</v>
+        <v>224</v>
       </c>
       <c r="E182" t="s">
-        <v>415</v>
+        <v>369</v>
       </c>
       <c r="F182" t="s">
         <v>12</v>
@@ -5633,13 +5627,13 @@
         <v>27</v>
       </c>
       <c r="C183" t="s">
-        <v>438</v>
+        <v>392</v>
       </c>
       <c r="D183" t="s">
-        <v>258</v>
+        <v>224</v>
       </c>
       <c r="E183" t="s">
-        <v>415</v>
+        <v>369</v>
       </c>
       <c r="F183" t="s">
         <v>12</v>
@@ -5653,13 +5647,13 @@
         <v>28</v>
       </c>
       <c r="C184" t="s">
-        <v>439</v>
+        <v>393</v>
       </c>
       <c r="D184" t="s">
-        <v>258</v>
+        <v>224</v>
       </c>
       <c r="E184" t="s">
-        <v>415</v>
+        <v>369</v>
       </c>
       <c r="F184" t="s">
         <v>12</v>
@@ -5673,13 +5667,13 @@
         <v>29</v>
       </c>
       <c r="C185" t="s">
-        <v>440</v>
+        <v>394</v>
       </c>
       <c r="D185" t="s">
-        <v>258</v>
+        <v>224</v>
       </c>
       <c r="E185" t="s">
-        <v>415</v>
+        <v>369</v>
       </c>
       <c r="F185" t="s">
         <v>12</v>
@@ -5693,13 +5687,13 @@
         <v>30</v>
       </c>
       <c r="C186" t="s">
-        <v>441</v>
+        <v>395</v>
       </c>
       <c r="D186" t="s">
-        <v>258</v>
+        <v>224</v>
       </c>
       <c r="E186" t="s">
-        <v>415</v>
+        <v>369</v>
       </c>
       <c r="F186" t="s">
         <v>12</v>
@@ -5722,67 +5716,67 @@
     </row>
     <row r="200" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E200" t="s">
-        <v>416</v>
+        <v>370</v>
       </c>
     </row>
     <row r="201" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E201" t="s">
-        <v>417</v>
+        <v>371</v>
       </c>
     </row>
     <row r="202" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E202" t="s">
-        <v>418</v>
+        <v>372</v>
       </c>
     </row>
     <row r="203" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E203" t="s">
-        <v>419</v>
+        <v>373</v>
       </c>
     </row>
     <row r="204" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E204" t="s">
-        <v>420</v>
+        <v>374</v>
       </c>
     </row>
     <row r="205" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E205" t="s">
-        <v>421</v>
+        <v>375</v>
       </c>
     </row>
     <row r="206" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E206" t="s">
-        <v>422</v>
+        <v>376</v>
       </c>
     </row>
     <row r="207" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E207" t="s">
-        <v>423</v>
+        <v>377</v>
       </c>
     </row>
     <row r="208" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E208" t="s">
-        <v>424</v>
+        <v>378</v>
       </c>
     </row>
     <row r="209" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E209" t="s">
-        <v>425</v>
+        <v>379</v>
       </c>
     </row>
     <row r="210" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E210" t="s">
-        <v>426</v>
+        <v>380</v>
       </c>
     </row>
     <row r="211" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E211" t="s">
-        <v>427</v>
+        <v>381</v>
       </c>
     </row>
     <row r="212" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E212" t="s">
-        <v>428</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>

</xml_diff>